<commit_message>
[박청아] Add - [AI] Staff가 Slot 1개 가지도록 추가
</commit_message>
<xml_diff>
--- a/Content/TableData/Staff.xlsx
+++ b/Content/TableData/Staff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F28DBA-C88B-4796-B170-41C52E4D121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE4416A-C8C4-4352-993D-2E30E9BDB010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25830" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5565" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>int32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,6 +120,14 @@
   </si>
   <si>
     <t>PathFile</t>
+  </si>
+  <si>
+    <t>int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SlotCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>int32</t>
@@ -451,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="H3" sqref="H3:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -462,7 +470,7 @@
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -485,13 +493,16 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -514,13 +525,16 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -542,14 +556,17 @@
       <c r="G3">
         <v>3000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
         <v>3001</v>
       </c>
-      <c r="I3">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -571,14 +588,17 @@
       <c r="G4">
         <v>3000</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
         <v>3001</v>
       </c>
-      <c r="I4">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -600,14 +620,17 @@
       <c r="G5">
         <v>3000</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
         <v>3002</v>
       </c>
-      <c r="I5">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -629,14 +652,17 @@
       <c r="G6">
         <v>4000</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
         <v>3003</v>
       </c>
-      <c r="I6">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -658,14 +684,17 @@
       <c r="G7">
         <v>4000</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
         <v>3004</v>
       </c>
-      <c r="I7">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -687,14 +716,17 @@
       <c r="G8">
         <v>3000</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
         <v>3005</v>
       </c>
-      <c r="I8">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -716,14 +748,17 @@
       <c r="G9">
         <v>3000</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
         <v>3006</v>
       </c>
-      <c r="I9">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -745,14 +780,17 @@
       <c r="G10">
         <v>3000</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
         <v>3001</v>
       </c>
-      <c r="I10">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -774,14 +812,17 @@
       <c r="G11">
         <v>4000</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
         <v>3002</v>
       </c>
-      <c r="I11">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -803,14 +844,17 @@
       <c r="G12">
         <v>4000</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
         <v>3003</v>
       </c>
-      <c r="I12">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -832,14 +876,17 @@
       <c r="G13">
         <v>3000</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
         <v>3004</v>
       </c>
-      <c r="I13">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -861,14 +908,17 @@
       <c r="G14">
         <v>4000</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
         <v>3005</v>
       </c>
-      <c r="I14">
-        <v>9001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>9001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -890,10 +940,13 @@
       <c r="G15">
         <v>3000</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
         <v>3006</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>9001</v>
       </c>
     </row>

</xml_diff>